<commit_message>
Update KRA page to enable review option based on reviewCycle
</commit_message>
<xml_diff>
--- a/server/key_result_data_export.xlsx
+++ b/server/key_result_data_export.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="20">
   <si>
     <t>period</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>Development</t>
+  </si>
+  <si>
+    <t/>
   </si>
 </sst>
 </file>
@@ -113,7 +116,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I13"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -200,7 +203,9 @@
       <c r="H4" t="n" s="0">
         <v>3.0</v>
       </c>
-      <c r="I4" s="0"/>
+      <c r="I4" t="n" s="0">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="s" s="0">
@@ -225,7 +230,9 @@
       <c r="H5" t="n" s="0">
         <v>3.0</v>
       </c>
-      <c r="I5" s="0"/>
+      <c r="I5" t="n" s="0">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="s" s="0">
@@ -248,9 +255,11 @@
         <v>11</v>
       </c>
       <c r="H6" t="n" s="0">
-        <v>2468.0</v>
-      </c>
-      <c r="I6" s="0"/>
+        <v>2.0</v>
+      </c>
+      <c r="I6" t="n" s="0">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="s" s="0">
@@ -267,15 +276,17 @@
         <v>12</v>
       </c>
       <c r="F7" t="n" s="0">
-        <v>10.0</v>
+        <v>20.0</v>
       </c>
       <c r="G7" t="s" s="0">
         <v>13</v>
       </c>
       <c r="H7" t="n" s="0">
-        <v>2468.0</v>
-      </c>
-      <c r="I7" s="0"/>
+        <v>2.0</v>
+      </c>
+      <c r="I7" t="n" s="0">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="s" s="0">
@@ -298,9 +309,11 @@
         <v>16</v>
       </c>
       <c r="H8" t="n" s="0">
-        <v>2468.0</v>
-      </c>
-      <c r="I8" s="0"/>
+        <v>2.0</v>
+      </c>
+      <c r="I8" t="n" s="0">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="s" s="0">
@@ -311,7 +324,7 @@
       </c>
       <c r="C9" s="0"/>
       <c r="D9" t="n" s="0">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E9" t="s" s="0">
         <v>10</v>
@@ -323,9 +336,11 @@
         <v>11</v>
       </c>
       <c r="H9" t="n" s="0">
-        <v>3690.0</v>
-      </c>
-      <c r="I9" s="0"/>
+        <v>5.0</v>
+      </c>
+      <c r="I9" t="n" s="0">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="s" s="0">
@@ -336,7 +351,7 @@
       </c>
       <c r="C10" s="0"/>
       <c r="D10" t="n" s="0">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E10" t="s" s="0">
         <v>12</v>
@@ -348,9 +363,11 @@
         <v>13</v>
       </c>
       <c r="H10" t="n" s="0">
-        <v>3690.0</v>
-      </c>
-      <c r="I10" s="0"/>
+        <v>5.0</v>
+      </c>
+      <c r="I10" t="n" s="0">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="s" s="0">
@@ -361,7 +378,7 @@
       </c>
       <c r="C11" s="0"/>
       <c r="D11" t="n" s="0">
-        <v>3.0</v>
+        <v>2.0</v>
       </c>
       <c r="E11" t="s" s="0">
         <v>15</v>
@@ -373,9 +390,11 @@
         <v>16</v>
       </c>
       <c r="H11" t="n" s="0">
-        <v>3690.0</v>
-      </c>
-      <c r="I11" s="0"/>
+        <v>10.0</v>
+      </c>
+      <c r="I11" t="n" s="0">
+        <v>1.0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="s" s="0">
@@ -403,6 +422,25 @@
       <c r="I12" t="n" s="0">
         <v>1.0</v>
       </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="B13" t="n" s="0">
+        <v>21.0</v>
+      </c>
+      <c r="C13" s="0"/>
+      <c r="D13" s="0"/>
+      <c r="E13" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="F13" s="0"/>
+      <c r="G13" t="s" s="0">
+        <v>19</v>
+      </c>
+      <c r="H13" s="0"/>
+      <c r="I13" s="0"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>